<commit_message>
manual annotation user satisfication & relevance
</commit_message>
<xml_diff>
--- a/evaluation_results.xlsx
+++ b/evaluation_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eviat\PycharmProjects\ConversationalAgent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A04864E-C9DE-4BEC-A79A-3A198808FA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD91C49-80DE-4D52-8EAA-282E052AD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>Input</t>
   </si>
@@ -192,13 +192,19 @@
   <si>
     <t>To cancel your order, please provide your order ID so I can assist you further.
 ```</t>
+  </si>
+  <si>
+    <t>User Satisfication</t>
+  </si>
+  <si>
+    <t>Relevance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +217,20 @@
       <sz val="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -220,7 +240,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -243,13 +263,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -554,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -565,9 +600,11 @@
     <col min="1" max="1" width="93.75" customWidth="1"/>
     <col min="2" max="2" width="109" customWidth="1"/>
     <col min="3" max="3" width="123.125" customWidth="1"/>
+    <col min="4" max="4" width="23.75" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +614,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -588,8 +631,14 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -599,8 +648,14 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -610,8 +665,14 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -621,8 +682,14 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -632,8 +699,14 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -643,8 +716,14 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -654,8 +733,14 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -665,8 +750,14 @@
       <c r="C9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -676,8 +767,14 @@
       <c r="C10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -687,8 +784,14 @@
       <c r="C11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -698,8 +801,14 @@
       <c r="C12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -709,8 +818,14 @@
       <c r="C13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -720,8 +835,14 @@
       <c r="C14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -731,8 +852,14 @@
       <c r="C15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -742,8 +869,14 @@
       <c r="C16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -753,8 +886,14 @@
       <c r="C17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -764,8 +903,14 @@
       <c r="C18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -775,8 +920,14 @@
       <c r="C19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -786,8 +937,14 @@
       <c r="C20" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -797,8 +954,14 @@
       <c r="C21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -808,8 +971,14 @@
       <c r="C22" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -819,8 +988,14 @@
       <c r="C23" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -830,8 +1005,14 @@
       <c r="C24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -841,8 +1022,14 @@
       <c r="C25" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -852,8 +1039,15 @@
       <c r="C26" t="s">
         <v>53</v>
       </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>